<commit_message>
Update ProdStarDay and ProdEndDay for Trout Lake
</commit_message>
<xml_diff>
--- a/TroutLake/ConfigurationInputsTrout.xlsx
+++ b/TroutLake/ConfigurationInputsTrout.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJF\Desktop\R\SOS\TroutLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="15720" windowHeight="5865"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ConfigurationInputsTrout" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -127,12 +132,24 @@
   </si>
   <si>
     <t>g/m2/yr</t>
+  </si>
+  <si>
+    <t>#ProductionPeriod</t>
+  </si>
+  <si>
+    <t>ProdStartDay</t>
+  </si>
+  <si>
+    <t>JulianDay</t>
+  </si>
+  <si>
+    <t>ProdEndDay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -445,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,6 +710,33 @@
         <v>35</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>330</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Trout ConfigInputs based on optimization
</commit_message>
<xml_diff>
--- a/TroutLake/ConfigurationInputsTrout.xlsx
+++ b/TroutLake/ConfigurationInputsTrout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -144,6 +144,24 @@
   </si>
   <si>
     <t>ProdEndDay</t>
+  </si>
+  <si>
+    <t>BurialFactor_R</t>
+  </si>
+  <si>
+    <t>BurialFactor_L</t>
+  </si>
+  <si>
+    <t>POC_lcR</t>
+  </si>
+  <si>
+    <t>POC_lcL</t>
+  </si>
+  <si>
+    <t>DOCR_RespParam</t>
+  </si>
+  <si>
+    <t>DOCL_RespParam</t>
   </si>
 </sst>
 </file>
@@ -462,17 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.875" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,168 +594,235 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>1.4696080000000001E-3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B12">
-        <v>0.77</v>
+        <v>8.3764389999999998E-4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.77</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>0.19</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0.19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21">
-        <v>0.01</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>1E-3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>0.17578609049999999</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>9.5980883999999995E-3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B26">
-        <v>27</v>
+        <v>1E-3</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>9.963455E-4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B28">
-        <v>105</v>
+        <v>0.12293787389999999</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.78708956070000002</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B29">
+      <c r="B35">
         <v>330</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C35" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>